<commit_message>
fix feature add employee by excel
</commit_message>
<xml_diff>
--- a/Backend/scripts/employee-import-template.xlsx
+++ b/Backend/scripts/employee-import-template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>staff</t>
+  </si>
+  <si>
+    <t>react,python,c++,javascript</t>
   </si>
   <si>
     <t>Jane Manager</t>
@@ -83,7 +86,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -93,6 +96,10 @@
     <font>
       <b/>
       <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
@@ -137,10 +144,10 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="top"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -365,7 +372,7 @@
     <col customWidth="1" min="6" max="6" width="17.14"/>
     <col customWidth="1" min="7" max="7" width="21.86"/>
     <col customWidth="1" min="8" max="8" width="24.0"/>
-    <col customWidth="1" min="9" max="26" width="8.71"/>
+    <col customWidth="1" min="9" max="9" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -393,57 +400,60 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>